<commit_message>
commit added new test and pages like logout page password reset page and test
</commit_message>
<xml_diff>
--- a/openkart2/testData/TestCaseInputData.xlsx
+++ b/openkart2/testData/TestCaseInputData.xlsx
@@ -5,36 +5,49 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EdurekaTrain23\openkart2\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepo\openkart2\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84431A40-0E46-47A8-95BC-12DF15F04CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A589EDD7-5787-4BF3-A3A1-5B380684756A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC001_Registration" sheetId="1" r:id="rId1"/>
     <sheet name="TC002" sheetId="2" r:id="rId2"/>
     <sheet name="TC003_Login" sheetId="9" r:id="rId3"/>
-    <sheet name="TC005_LoginDDT" sheetId="10" r:id="rId4"/>
-    <sheet name="TC004" sheetId="7" r:id="rId5"/>
-    <sheet name="TC005" sheetId="8" r:id="rId6"/>
-    <sheet name="TC003" sheetId="3" r:id="rId7"/>
-    <sheet name="TC006" sheetId="6" r:id="rId8"/>
-    <sheet name="TC007" sheetId="4" r:id="rId9"/>
-    <sheet name="TC008" sheetId="5" r:id="rId10"/>
+    <sheet name="TC006_Logout" sheetId="11" r:id="rId4"/>
+    <sheet name="TC007_PasswordResetMail" sheetId="12" r:id="rId5"/>
+    <sheet name="TC005_LoginDDT" sheetId="10" r:id="rId6"/>
+    <sheet name="TC004" sheetId="7" r:id="rId7"/>
+    <sheet name="TC005" sheetId="8" r:id="rId8"/>
+    <sheet name="TC003" sheetId="3" r:id="rId9"/>
+    <sheet name="TC006" sheetId="6" r:id="rId10"/>
+    <sheet name="TC007" sheetId="4" r:id="rId11"/>
+    <sheet name="TC008" sheetId="5" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="336">
   <si>
     <t>password</t>
   </si>
@@ -1024,6 +1037,24 @@
   </si>
   <si>
     <t>Invalid</t>
+  </si>
+  <si>
+    <t>logoutmsg</t>
+  </si>
+  <si>
+    <t>You have been logged off your account. It is now s</t>
+  </si>
+  <si>
+    <t>HeaderTxt</t>
+  </si>
+  <si>
+    <t>Forgot Your Password?</t>
+  </si>
+  <si>
+    <t>An email with a confirmation link has been sent your email address.</t>
+  </si>
+  <si>
+    <t>EmailSuccess</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1169,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1158,6 +1189,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1534,1424 +1568,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42142EAE-831F-4435-B56A-808DC4DD1E23}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{0918B3E3-6757-4E3D-B311-65476AD179D7}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{7A29181E-E795-4C25-AC1C-D120EFCE91A1}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{D5AD620E-80E8-4788-8C3D-64A0E8D16289}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{367DAAD5-4407-41E2-9787-C99E2E11DF99}"/>
-    <hyperlink ref="D4" r:id="rId5" xr:uid="{C205BB12-DB45-4B9E-AECB-A7961084A6DB}"/>
-    <hyperlink ref="C4" r:id="rId6" xr:uid="{BD353BF9-7957-408A-AC1F-0FB02668A12F}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A60C306-163A-4680-9628-73989D56D839}">
-  <dimension ref="A1:AH4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC1" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>301</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" t="s">
-        <v>80</v>
-      </c>
-      <c r="O2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="S2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>227</v>
-      </c>
-      <c r="B3" t="s">
-        <v>299</v>
-      </c>
-      <c r="C3" t="s">
-        <v>299</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="M3" t="s">
-        <v>91</v>
-      </c>
-      <c r="N3" t="s">
-        <v>92</v>
-      </c>
-      <c r="O3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="S3" t="s">
-        <v>95</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>300</v>
-      </c>
-      <c r="C4" t="s">
-        <v>300</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="M4" t="s">
-        <v>80</v>
-      </c>
-      <c r="N4" t="s">
-        <v>103</v>
-      </c>
-      <c r="O4" t="s">
-        <v>17</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" t="s">
-        <v>104</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="AC4" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{BA1B005B-8529-4140-9DD5-53DE3BF91F2F}"/>
-    <hyperlink ref="K3" r:id="rId2" xr:uid="{32DBF9BB-D42C-47BC-B7BD-56AD8B9D8E72}"/>
-    <hyperlink ref="K4" r:id="rId3" xr:uid="{F8AD5BBA-FF92-43EE-8B20-4F8B03EB1500}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CCE5BE-4413-40F1-AF35-0DF49666642C}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>326</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>323</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{BA2A2F2F-3049-4FEB-99F6-20163042B19A}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{DCDEA8C0-0610-4173-8DD8-6D26769CAB4A}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{BFE72E43-58A8-413C-8F1F-544D9662B009}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7470CB73-61C9-4590-BAD9-7BAC1A21F6AD}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>326</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>328</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{268C9AE2-574E-49E8-B8B6-A8F502529ACC}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{3D714B93-FE18-4160-82F3-2EC037AC4C1E}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{6505F1D2-3DA7-43BA-9464-F03F79E9EF30}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF14B62D-6D1A-48C0-A5C7-25F1D71FF1AC}">
-  <dimension ref="A1:Q4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F1" t="s">
-        <v>263</v>
-      </c>
-      <c r="G1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" t="s">
-        <v>296</v>
-      </c>
-      <c r="I1" t="s">
-        <v>264</v>
-      </c>
-      <c r="J1" t="s">
-        <v>275</v>
-      </c>
-      <c r="K1" t="s">
-        <v>276</v>
-      </c>
-      <c r="L1" t="s">
-        <v>277</v>
-      </c>
-      <c r="M1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>279</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E2" t="s">
-        <v>298</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="H2" t="s">
-        <v>298</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="M2" t="s">
-        <v>204</v>
-      </c>
-      <c r="N2" t="s">
-        <v>103</v>
-      </c>
-      <c r="O2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C3" t="s">
-        <v>281</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E3" t="s">
-        <v>298</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="H3" t="s">
-        <v>298</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="M3" t="s">
-        <v>74</v>
-      </c>
-      <c r="N3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="H4" t="s">
-        <v>298</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="M4" t="s">
-        <v>221</v>
-      </c>
-      <c r="N4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{C67FA3FA-43E6-444D-9BF8-05E8B09E0D1B}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{59FB9A9D-0A91-4A55-A986-F722CE84F2FB}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{28B266C3-B4FC-443E-98FA-E9865ADC48BD}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD93B10-87F1-46A9-9AE3-82EFB8913123}">
-  <dimension ref="A1:T4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="D1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F1" t="s">
-        <v>263</v>
-      </c>
-      <c r="G1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" t="s">
-        <v>296</v>
-      </c>
-      <c r="I1" t="s">
-        <v>264</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>279</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E2" t="s">
-        <v>298</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="H2" t="s">
-        <v>298</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="M2" t="s">
-        <v>204</v>
-      </c>
-      <c r="N2" t="s">
-        <v>103</v>
-      </c>
-      <c r="O2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>286</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="S2" t="s">
-        <v>288</v>
-      </c>
-      <c r="T2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C3" t="s">
-        <v>281</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E3" t="s">
-        <v>298</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="H3" t="s">
-        <v>298</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="M3" t="s">
-        <v>74</v>
-      </c>
-      <c r="N3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>286</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="S3" t="s">
-        <v>291</v>
-      </c>
-      <c r="T3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="H4" t="s">
-        <v>298</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="M4" t="s">
-        <v>221</v>
-      </c>
-      <c r="N4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>286</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="S4" t="s">
-        <v>293</v>
-      </c>
-      <c r="T4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{52173C14-9933-41A1-9B87-11C004384390}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{728C6A92-D096-4099-863A-E30B8BAFFE36}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{61FC52E2-327D-48C1-9C5E-3971C5DAAEB7}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8342DA-1C84-4677-A1EF-5DFEEC2D3B58}">
-  <dimension ref="A1:O4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="G2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" t="s">
-        <v>133</v>
-      </c>
-      <c r="O2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="G3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="N3" t="s">
-        <v>108</v>
-      </c>
-      <c r="O3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="G4" t="s">
-        <v>143</v>
-      </c>
-      <c r="H4" t="s">
-        <v>146</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="N4" t="s">
-        <v>147</v>
-      </c>
-      <c r="O4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{78CBDD1B-CA0F-4E58-B4AD-0CE2C31917F1}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{612D1BE1-6FD5-49F8-874C-04BC824DA0F1}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{B655D5F9-69D6-47A1-B82D-081C3ADCFEA1}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B1DC76-5196-4419-BCBD-1EDCAF41A15F}">
   <dimension ref="A1:AR4"/>
   <sheetViews>
@@ -3531,7 +2147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9668C667-407F-49A8-B960-29510C1FF716}">
   <dimension ref="A1:N4"/>
   <sheetViews>
@@ -3736,4 +2352,1512 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42142EAE-831F-4435-B56A-808DC4DD1E23}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{0918B3E3-6757-4E3D-B311-65476AD179D7}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{7A29181E-E795-4C25-AC1C-D120EFCE91A1}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{D5AD620E-80E8-4788-8C3D-64A0E8D16289}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{367DAAD5-4407-41E2-9787-C99E2E11DF99}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{C205BB12-DB45-4B9E-AECB-A7961084A6DB}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{BD353BF9-7957-408A-AC1F-0FB02668A12F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A60C306-163A-4680-9628-73989D56D839}">
+  <dimension ref="A1:AH4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="S2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M3" t="s">
+        <v>91</v>
+      </c>
+      <c r="N3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="S3" t="s">
+        <v>95</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" t="s">
+        <v>103</v>
+      </c>
+      <c r="O4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" t="s">
+        <v>104</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{BA1B005B-8529-4140-9DD5-53DE3BF91F2F}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{32DBF9BB-D42C-47BC-B7BD-56AD8B9D8E72}"/>
+    <hyperlink ref="K4" r:id="rId3" xr:uid="{F8AD5BBA-FF92-43EE-8B20-4F8B03EB1500}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CCE5BE-4413-40F1-AF35-0DF49666642C}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{BA2A2F2F-3049-4FEB-99F6-20163042B19A}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{DCDEA8C0-0610-4173-8DD8-6D26769CAB4A}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{BFE72E43-58A8-413C-8F1F-544D9662B009}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94516573-E601-4FB3-AFAD-6648253C9BA4}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>331</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{25A1895C-12C8-4184-B725-1BA7AAD66C81}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF8D3F6-1DC4-49A3-A0A0-5BD29515FF3F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="61" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4F9CE4A7-4100-4E57-A786-D2B49BE1EB69}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7470CB73-61C9-4590-BAD9-7BAC1A21F6AD}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{268C9AE2-574E-49E8-B8B6-A8F502529ACC}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{3D714B93-FE18-4160-82F3-2EC037AC4C1E}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{6505F1D2-3DA7-43BA-9464-F03F79E9EF30}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF14B62D-6D1A-48C0-A5C7-25F1D71FF1AC}">
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" t="s">
+        <v>296</v>
+      </c>
+      <c r="I1" t="s">
+        <v>264</v>
+      </c>
+      <c r="J1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K1" t="s">
+        <v>276</v>
+      </c>
+      <c r="L1" t="s">
+        <v>277</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H2" t="s">
+        <v>298</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="M2" t="s">
+        <v>204</v>
+      </c>
+      <c r="N2" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H3" t="s">
+        <v>298</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="M3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H4" t="s">
+        <v>298</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="M4" t="s">
+        <v>221</v>
+      </c>
+      <c r="N4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C67FA3FA-43E6-444D-9BF8-05E8B09E0D1B}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{59FB9A9D-0A91-4A55-A986-F722CE84F2FB}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{28B266C3-B4FC-443E-98FA-E9865ADC48BD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD93B10-87F1-46A9-9AE3-82EFB8913123}">
+  <dimension ref="A1:T4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" t="s">
+        <v>296</v>
+      </c>
+      <c r="I1" t="s">
+        <v>264</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H2" t="s">
+        <v>298</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="M2" t="s">
+        <v>204</v>
+      </c>
+      <c r="N2" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>286</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="S2" t="s">
+        <v>288</v>
+      </c>
+      <c r="T2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H3" t="s">
+        <v>298</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="M3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>286</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="S3" t="s">
+        <v>291</v>
+      </c>
+      <c r="T3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H4" t="s">
+        <v>298</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="M4" t="s">
+        <v>221</v>
+      </c>
+      <c r="N4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>286</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="S4" t="s">
+        <v>293</v>
+      </c>
+      <c r="T4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{52173C14-9933-41A1-9B87-11C004384390}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{728C6A92-D096-4099-863A-E30B8BAFFE36}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{61FC52E2-327D-48C1-9C5E-3971C5DAAEB7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8342DA-1C84-4677-A1EF-5DFEEC2D3B58}">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" t="s">
+        <v>130</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" t="s">
+        <v>133</v>
+      </c>
+      <c r="O2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="N3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N4" t="s">
+        <v>147</v>
+      </c>
+      <c r="O4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{78CBDD1B-CA0F-4E58-B4AD-0CE2C31917F1}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{612D1BE1-6FD5-49F8-874C-04BC824DA0F1}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{B655D5F9-69D6-47A1-B82D-081C3ADCFEA1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit 5-added randon methods and also changed the account registration page
</commit_message>
<xml_diff>
--- a/openkart2/testData/TestCaseInputData.xlsx
+++ b/openkart2/testData/TestCaseInputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepo\openkart2\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A589EDD7-5787-4BF3-A3A1-5B380684756A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A124945F-BD5E-48C0-8850-41BBFDE8B5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC001_Registration" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="333">
   <si>
     <t>password</t>
   </si>
@@ -964,9 +964,6 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>EmailID</t>
-  </si>
-  <si>
     <t>TelephoneNumber</t>
   </si>
   <si>
@@ -1004,12 +1001,6 @@
   </si>
   <si>
     <t>8985998545</t>
-  </si>
-  <si>
-    <t>Bashn9085e67568@gmail.com</t>
-  </si>
-  <si>
-    <t>Narinder37977@gmail.com</t>
   </si>
   <si>
     <t>UserEmail</t>
@@ -1473,22 +1464,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>303</v>
       </c>
@@ -1504,66 +1494,53 @@
       <c r="E1" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="16" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>308</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="B2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>309</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>311</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" t="s">
         <v>313</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E3" t="s">
         <v>313</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>310</v>
-      </c>
-      <c r="B3" t="s">
-        <v>312</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E3" t="s">
-        <v>314</v>
-      </c>
-      <c r="F3" t="s">
-        <v>314</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>316</v>
+      <c r="F3" s="14" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{83C774F3-3025-4D70-B442-1183795E639F}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{E518B873-F50A-4920-BC26-B3FF2C51F264}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2934,42 +2911,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -2999,24 +2976,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -3031,9 +3008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF8D3F6-1DC4-49A3-A0A0-5BD29515FF3F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3047,21 +3022,21 @@
         <v>151</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>332</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -3087,57 +3062,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>